<commit_message>
Agregado el array en el Excel file
</commit_message>
<xml_diff>
--- a/testData/studentData.xlsx
+++ b/testData/studentData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dagoberto\eclipse-workspace\Students.APIAutomation\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845A4796-A745-49BF-AF1A-A051ADE1B954}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB42A42-3156-4035-98B3-2D4BDF41F214}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>courses</t>
+  </si>
+  <si>
+    <t>java,c</t>
+  </si>
+  <si>
+    <t>js,php</t>
+  </si>
+  <si>
+    <t>c++,java</t>
   </si>
 </sst>
 </file>
@@ -372,15 +384,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -393,8 +405,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -407,8 +422,11 @@
       <c r="D2">
         <v>123132</v>
       </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -421,8 +439,11 @@
       <c r="D3">
         <v>43546</v>
       </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -434,6 +455,9 @@
       </c>
       <c r="D4">
         <v>78778</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>